<commit_message>
gestion des erreur utilsateur
</commit_message>
<xml_diff>
--- a/code/public/assets/excels/creerCompte.xlsx
+++ b/code/public/assets/excels/creerCompte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoisgraux/GITLAB/SAE/projet-sae-s3/code/public/assets/excels file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoisgraux/GITLAB/SAE/projet-sae-s3/code/public/assets/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC9132CF-893D-744E-9221-90CC9D0DF107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3829568B-D9C6-7E4C-BDEF-9372C56E8C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17440" xr2:uid="{D1189E1C-C832-0D44-B26C-D3B8DD5BD73B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>nom</t>
   </si>
@@ -50,7 +50,10 @@
     <t>prenom</t>
   </si>
   <si>
-    <t>type compte</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>aled</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E786A3-1B6D-7B42-BD01-CEFC4978B9DB}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,6 +430,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modif nom fichier API + modif nom route associé
</commit_message>
<xml_diff>
--- a/code/public/assets/excels/creerCompte.xlsx
+++ b/code/public/assets/excels/creerCompte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francoisgraux/GITLAB/SAE/projet-sae-s3/code/public/assets/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G1S3\SAE\projet-sae-s3\code\public\assets\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3829568B-D9C6-7E4C-BDEF-9372C56E8C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CFB52D-BCF9-49BB-AA13-129CACB1BB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17440" xr2:uid="{D1189E1C-C832-0D44-B26C-D3B8DD5BD73B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1189E1C-C832-0D44-B26C-D3B8DD5BD73B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nom</t>
   </si>
@@ -51,9 +49,6 @@
   </si>
   <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>aled</t>
   </si>
 </sst>
 </file>
@@ -109,7 +104,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -405,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E786A3-1B6D-7B42-BD01-CEFC4978B9DB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -430,23 +425,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>